<commit_message>
Add binified, year-in-review map
</commit_message>
<xml_diff>
--- a/csv/UNI.xlsx
+++ b/csv/UNI.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="23913"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="2000" yWindow="460" windowWidth="25040" windowHeight="15500" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="380" yWindow="0" windowWidth="22580" windowHeight="15500" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="New Crimes" sheetId="2" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="587" uniqueCount="137">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="670" uniqueCount="166">
   <si>
     <t>date</t>
   </si>
@@ -356,49 +356,7 @@
     <t>13:28:00</t>
   </si>
   <si>
-    <t>13-476</t>
-  </si>
-  <si>
     <t>Hagemann Hall</t>
-  </si>
-  <si>
-    <t>10/15/2013 0000- 10/15/2013 2359</t>
-  </si>
-  <si>
-    <t>13-478</t>
-  </si>
-  <si>
-    <t>10/30/2013 2113</t>
-  </si>
-  <si>
-    <t>10/30/2013 1830 - 10/30/2013 2040</t>
-  </si>
-  <si>
-    <t>13-480</t>
-  </si>
-  <si>
-    <t>10/31/2013 1654</t>
-  </si>
-  <si>
-    <t>13-487</t>
-  </si>
-  <si>
-    <t>11/01/2013 1313</t>
-  </si>
-  <si>
-    <t>13-493</t>
-  </si>
-  <si>
-    <t>11/04/2013 1101</t>
-  </si>
-  <si>
-    <t>11/02/2013 0800 / 11/03/2013 2000</t>
-  </si>
-  <si>
-    <t>13-498</t>
-  </si>
-  <si>
-    <t>11/06/2013 1433</t>
   </si>
   <si>
     <t>N/A</t>
@@ -433,6 +391,135 @@
   <si>
     <t>14:33:00</t>
   </si>
+  <si>
+    <t>11/09/2013</t>
+  </si>
+  <si>
+    <t>18:09:00</t>
+  </si>
+  <si>
+    <t>11/11/2013</t>
+  </si>
+  <si>
+    <t>09:19:00</t>
+  </si>
+  <si>
+    <t>11/12/2013</t>
+  </si>
+  <si>
+    <t>09:04:00</t>
+  </si>
+  <si>
+    <t>11/18/2013</t>
+  </si>
+  <si>
+    <t>15:00:00</t>
+  </si>
+  <si>
+    <t>11/20/2013</t>
+  </si>
+  <si>
+    <t>08:17:00</t>
+  </si>
+  <si>
+    <t>15:03:00</t>
+  </si>
+  <si>
+    <t>Curris Business Building</t>
+  </si>
+  <si>
+    <t>11/22/2013</t>
+  </si>
+  <si>
+    <t>09:48:00</t>
+  </si>
+  <si>
+    <t>11/23/2013</t>
+  </si>
+  <si>
+    <t>13:17:00</t>
+  </si>
+  <si>
+    <t>16:14:00</t>
+  </si>
+  <si>
+    <t>11/25/2013</t>
+  </si>
+  <si>
+    <t>14:10:00</t>
+  </si>
+  <si>
+    <t>12/08/2013</t>
+  </si>
+  <si>
+    <t>15:35:00</t>
+  </si>
+  <si>
+    <t>12/15/2013</t>
+  </si>
+  <si>
+    <t>14:11:00</t>
+  </si>
+  <si>
+    <t>13-595</t>
+  </si>
+  <si>
+    <t>12/16/2013 1037</t>
+  </si>
+  <si>
+    <t>13-596</t>
+  </si>
+  <si>
+    <t>West Gym</t>
+  </si>
+  <si>
+    <t>12/16/2013 1625</t>
+  </si>
+  <si>
+    <t>12/12/2013 1100 - 12/12/2013 1115</t>
+  </si>
+  <si>
+    <t>12/16/2013 1038</t>
+  </si>
+  <si>
+    <t>13-603</t>
+  </si>
+  <si>
+    <t>12/18/2013 1409</t>
+  </si>
+  <si>
+    <t>12/05/2013 0000 - 12/17/2013 2359</t>
+  </si>
+  <si>
+    <t>13-608</t>
+  </si>
+  <si>
+    <t>12/20/2013 1442</t>
+  </si>
+  <si>
+    <t>12/12/2013 1800 - 12/12/2013 1830</t>
+  </si>
+  <si>
+    <t>12/16/2013</t>
+  </si>
+  <si>
+    <t>10:37:00</t>
+  </si>
+  <si>
+    <t>16:25:00</t>
+  </si>
+  <si>
+    <t>12/18/2013</t>
+  </si>
+  <si>
+    <t>14:09:00</t>
+  </si>
+  <si>
+    <t>12/20/2013</t>
+  </si>
+  <si>
+    <t>14:42:00</t>
+  </si>
 </sst>
 </file>
 
@@ -441,7 +528,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="[h]:mm:ss;@"/>
   </numFmts>
-  <fonts count="9" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -505,6 +592,11 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="13"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -523,7 +615,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="91">
+  <cellStyleXfs count="137">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -615,8 +707,54 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -656,8 +794,10 @@
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="91">
+  <cellStyles count="137">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -703,6 +843,29 @@
     <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -748,6 +911,29 @@
     <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="1">
@@ -1088,10 +1274,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O7"/>
+  <dimension ref="A1:P7"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2:O7"/>
+    <sheetView topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:O5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="20" x14ac:dyDescent="0"/>
@@ -1112,7 +1298,7 @@
     <col min="16" max="16384" width="10.83203125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" s="2" customFormat="1" ht="18">
+    <row r="1" spans="1:16" s="2" customFormat="1" ht="18">
       <c r="A1" s="11" t="s">
         <v>59</v>
       </c>
@@ -1159,21 +1345,21 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:15" ht="18">
+    <row r="2" spans="1:16" ht="18">
       <c r="A2" t="s">
-        <v>111</v>
+        <v>146</v>
       </c>
       <c r="B2" t="s">
-        <v>46</v>
+        <v>8</v>
       </c>
       <c r="C2" t="s">
-        <v>112</v>
-      </c>
-      <c r="D2" s="4">
-        <v>40115</v>
+        <v>36</v>
+      </c>
+      <c r="D2" t="s">
+        <v>147</v>
       </c>
       <c r="E2" t="s">
-        <v>113</v>
+        <v>152</v>
       </c>
       <c r="F2" t="s">
         <v>10</v>
@@ -1181,22 +1367,24 @@
       <c r="G2" s="15" t="s">
         <v>55</v>
       </c>
-      <c r="H2" s="16" t="s">
-        <v>107</v>
-      </c>
-      <c r="I2" s="10" t="s">
-        <v>126</v>
+      <c r="H2" s="16" t="str">
+        <f>LEFT(D2, 10)</f>
+        <v>12/16/2013</v>
+      </c>
+      <c r="I2" s="10" t="str">
+        <f t="shared" ref="I2" si="0">CONCATENATE(REPLACE(RIGHT(D2,4),3,0,":"), ":00")</f>
+        <v>10:37:00</v>
       </c>
       <c r="J2" s="10" t="str">
-        <f t="shared" ref="J2:J7" si="0">B2</f>
-        <v>Sexual Assault</v>
+        <f t="shared" ref="J2" si="1">B2</f>
+        <v>Theft</v>
       </c>
       <c r="K2" s="10" t="str">
-        <f t="shared" ref="K2:K7" si="1">C2</f>
-        <v>Hagemann Hall</v>
+        <f t="shared" ref="K2" si="2">C2</f>
+        <v>Dancer Hall</v>
       </c>
       <c r="L2" s="10" t="str">
-        <f t="shared" ref="L2:L3" si="2">F2</f>
+        <f t="shared" ref="L2" si="3">F2</f>
         <v>Open</v>
       </c>
       <c r="M2" s="10" t="s">
@@ -1204,28 +1392,28 @@
       </c>
       <c r="N2" s="10">
         <f>VLOOKUP($C2, Locations!$A:$C, 2, FALSE)</f>
-        <v>42.512416000000002</v>
+        <v>42.518335</v>
       </c>
       <c r="O2" s="10">
         <f>VLOOKUP($C2, Locations!$A:$C, 3, FALSE)</f>
-        <v>-92.464008000000007</v>
+        <v>-92.461462999999995</v>
       </c>
     </row>
-    <row r="3" spans="1:15" ht="31">
+    <row r="3" spans="1:16" ht="18">
       <c r="A3" t="s">
-        <v>114</v>
+        <v>148</v>
       </c>
       <c r="B3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="6" t="s">
-        <v>52</v>
+      <c r="C3" t="s">
+        <v>149</v>
       </c>
       <c r="D3" t="s">
-        <v>115</v>
+        <v>150</v>
       </c>
       <c r="E3" t="s">
-        <v>116</v>
+        <v>151</v>
       </c>
       <c r="F3" t="s">
         <v>10</v>
@@ -1234,23 +1422,23 @@
         <v>55</v>
       </c>
       <c r="H3" s="16" t="str">
-        <f t="shared" ref="H3:H7" si="3">LEFT(D3, 10)</f>
-        <v>10/30/2013</v>
+        <f t="shared" ref="H3:H5" si="4">LEFT(D3, 10)</f>
+        <v>12/16/2013</v>
       </c>
       <c r="I3" s="10" t="str">
-        <f t="shared" ref="I3:I7" si="4">CONCATENATE(REPLACE(RIGHT(D3,4),3,0,":"), ":00")</f>
-        <v>21:13:00</v>
+        <f t="shared" ref="I3:I5" si="5">CONCATENATE(REPLACE(RIGHT(D3,4),3,0,":"), ":00")</f>
+        <v>16:25:00</v>
       </c>
       <c r="J3" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="J3:J5" si="6">B3</f>
         <v>Theft</v>
       </c>
       <c r="K3" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Innovative Teaching and Technical Center</v>
+        <f t="shared" ref="K3:K5" si="7">C3</f>
+        <v>West Gym</v>
       </c>
       <c r="L3" s="10" t="str">
-        <f t="shared" si="2"/>
+        <f t="shared" ref="L3:L5" si="8">F3</f>
         <v>Open</v>
       </c>
       <c r="M3" s="10" t="s">
@@ -1258,28 +1446,29 @@
       </c>
       <c r="N3" s="10">
         <f>VLOOKUP($C3, Locations!$A:$C, 2, FALSE)</f>
-        <v>42.515520000000002</v>
+        <v>42.513128999999999</v>
       </c>
       <c r="O3" s="10">
         <f>VLOOKUP($C3, Locations!$A:$C, 3, FALSE)</f>
-        <v>-92.459224000000006</v>
-      </c>
+        <v>-92.465681000000004</v>
+      </c>
+      <c r="P3"/>
     </row>
-    <row r="4" spans="1:15" ht="18">
+    <row r="4" spans="1:16" ht="18">
       <c r="A4" t="s">
-        <v>117</v>
+        <v>153</v>
       </c>
       <c r="B4" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="6" t="s">
-        <v>53</v>
+      <c r="C4" s="20" t="s">
+        <v>42</v>
       </c>
       <c r="D4" t="s">
-        <v>118</v>
+        <v>154</v>
       </c>
       <c r="E4" t="s">
-        <v>118</v>
+        <v>155</v>
       </c>
       <c r="F4" t="s">
         <v>10</v>
@@ -1288,23 +1477,23 @@
         <v>55</v>
       </c>
       <c r="H4" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>10/31/2013</v>
+        <f t="shared" si="4"/>
+        <v>12/18/2013</v>
       </c>
       <c r="I4" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>16:54:00</v>
+        <f t="shared" si="5"/>
+        <v>14:09:00</v>
       </c>
       <c r="J4" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Theft</v>
       </c>
       <c r="K4" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Gallagher Bluedorn</v>
+        <f t="shared" si="7"/>
+        <v>Rod Library</v>
       </c>
       <c r="L4" s="10" t="str">
-        <f t="shared" ref="L4:L7" si="5">F4</f>
+        <f t="shared" si="8"/>
         <v>Open</v>
       </c>
       <c r="M4" s="10" t="s">
@@ -1312,28 +1501,29 @@
       </c>
       <c r="N4" s="10">
         <f>VLOOKUP($C4, Locations!$A:$C, 2, FALSE)</f>
-        <v>42.510885000000002</v>
+        <v>42.514471</v>
       </c>
       <c r="O4" s="10">
         <f>VLOOKUP($C4, Locations!$A:$C, 3, FALSE)</f>
-        <v>-92.461005</v>
-      </c>
+        <v>-92.459536</v>
+      </c>
+      <c r="P4"/>
     </row>
-    <row r="5" spans="1:15" ht="18">
+    <row r="5" spans="1:16" ht="18">
       <c r="A5" t="s">
-        <v>119</v>
+        <v>156</v>
       </c>
       <c r="B5" t="s">
         <v>8</v>
       </c>
       <c r="C5" t="s">
-        <v>127</v>
+        <v>45</v>
       </c>
       <c r="D5" t="s">
-        <v>120</v>
+        <v>157</v>
       </c>
       <c r="E5" t="s">
-        <v>120</v>
+        <v>158</v>
       </c>
       <c r="F5" t="s">
         <v>10</v>
@@ -1342,23 +1532,23 @@
         <v>55</v>
       </c>
       <c r="H5" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>11/01/2013</v>
+        <f t="shared" si="4"/>
+        <v>12/20/2013</v>
       </c>
       <c r="I5" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>13:13:00</v>
+        <f t="shared" si="5"/>
+        <v>14:42:00</v>
       </c>
       <c r="J5" s="10" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" si="6"/>
         <v>Theft</v>
       </c>
       <c r="K5" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Gilchrist Hall</v>
+        <f t="shared" si="7"/>
+        <v>Noehren Hall</v>
       </c>
       <c r="L5" s="10" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="8"/>
         <v>Open</v>
       </c>
       <c r="M5" s="10" t="s">
@@ -1366,114 +1556,35 @@
       </c>
       <c r="N5" s="10">
         <f>VLOOKUP($C5, Locations!$A:$C, 2, FALSE)</f>
-        <v>42.51247</v>
+        <v>42.511201</v>
       </c>
       <c r="O5" s="10">
         <f>VLOOKUP($C5, Locations!$A:$C, 3, FALSE)</f>
-        <v>-92.459719000000007</v>
-      </c>
+        <v>-92.464398000000003</v>
+      </c>
+      <c r="P5"/>
     </row>
-    <row r="6" spans="1:15">
-      <c r="A6" t="s">
-        <v>121</v>
-      </c>
-      <c r="B6" t="s">
-        <v>8</v>
-      </c>
-      <c r="C6" t="s">
-        <v>41</v>
-      </c>
-      <c r="D6" t="s">
-        <v>122</v>
-      </c>
-      <c r="E6" t="s">
-        <v>123</v>
-      </c>
-      <c r="F6" t="s">
-        <v>10</v>
-      </c>
-      <c r="H6" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>11/04/2013</v>
-      </c>
-      <c r="I6" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>11:01:00</v>
-      </c>
-      <c r="J6" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>Theft</v>
-      </c>
-      <c r="K6" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>UNI Dome</v>
-      </c>
-      <c r="L6" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v>Open</v>
-      </c>
-      <c r="M6" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N6" s="10">
-        <f>VLOOKUP($C6, Locations!$A:$C, 2, FALSE)</f>
-        <v>42.515762000000002</v>
-      </c>
-      <c r="O6" s="10">
-        <f>VLOOKUP($C6, Locations!$A:$C, 3, FALSE)</f>
-        <v>-92.467191999999997</v>
-      </c>
+    <row r="6" spans="1:16">
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6"/>
+      <c r="K6"/>
+      <c r="L6"/>
+      <c r="M6"/>
+      <c r="N6"/>
+      <c r="O6"/>
+      <c r="P6"/>
     </row>
-    <row r="7" spans="1:15">
-      <c r="A7" t="s">
-        <v>124</v>
-      </c>
-      <c r="B7" t="s">
-        <v>8</v>
-      </c>
-      <c r="C7" t="s">
-        <v>47</v>
-      </c>
-      <c r="D7" t="s">
-        <v>125</v>
-      </c>
-      <c r="E7" t="s">
-        <v>125</v>
-      </c>
-      <c r="F7" t="s">
-        <v>10</v>
-      </c>
-      <c r="H7" s="16" t="str">
-        <f t="shared" si="3"/>
-        <v>11/06/2013</v>
-      </c>
-      <c r="I7" s="10" t="str">
-        <f t="shared" si="4"/>
-        <v>14:33:00</v>
-      </c>
-      <c r="J7" s="10" t="str">
-        <f t="shared" si="0"/>
-        <v>Theft</v>
-      </c>
-      <c r="K7" s="10" t="str">
-        <f t="shared" si="1"/>
-        <v>Roth Hall</v>
-      </c>
-      <c r="L7" s="10" t="str">
-        <f t="shared" si="5"/>
-        <v>Open</v>
-      </c>
-      <c r="M7" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="N7" s="10">
-        <f>VLOOKUP($C7, Locations!$A:$C, 2, FALSE)</f>
-        <v>42.508200000000002</v>
-      </c>
-      <c r="O7" s="10">
-        <f>VLOOKUP($C7, Locations!$A:$C, 3, FALSE)</f>
-        <v>-92.450855000000004</v>
-      </c>
+    <row r="7" spans="1:16">
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7"/>
+      <c r="K7"/>
+      <c r="L7"/>
+      <c r="M7"/>
+      <c r="N7"/>
+      <c r="O7"/>
+      <c r="P7"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -1488,10 +1599,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:XFD45"/>
+  <dimension ref="A1:XFD47"/>
   <sheetViews>
     <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1635,7 +1746,7 @@
     </row>
     <row r="13" spans="1:3">
       <c r="A13" s="17" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="B13" s="20">
         <v>42.51247</v>
@@ -1646,7 +1757,7 @@
     </row>
     <row r="14" spans="1:3">
       <c r="A14" s="17" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B14" s="22">
         <v>42.512416000000002</v>
@@ -18377,6 +18488,28 @@
         <v>-92.459059999999994</v>
       </c>
     </row>
+    <row r="46" spans="1:16384">
+      <c r="A46" t="s">
+        <v>134</v>
+      </c>
+      <c r="B46" s="23">
+        <v>42.513953000000001</v>
+      </c>
+      <c r="C46">
+        <v>-92.461827999999997</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16384" ht="16">
+      <c r="A47" s="6" t="s">
+        <v>149</v>
+      </c>
+      <c r="B47" s="24">
+        <v>42.513128999999999</v>
+      </c>
+      <c r="C47">
+        <v>-92.465681000000004</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="A2:XFD45">
     <sortCondition ref="A1"/>
@@ -18395,10 +18528,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H102"/>
+  <dimension ref="A1:H118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A67" workbookViewId="0">
-      <selection activeCell="E90" sqref="E90"/>
+    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
+      <selection activeCell="A115" sqref="A115:H118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -20914,13 +21047,13 @@
         <v>107</v>
       </c>
       <c r="B97" s="5" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
       <c r="C97" t="s">
         <v>46</v>
       </c>
       <c r="D97" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E97" t="s">
         <v>10</v>
@@ -20940,7 +21073,7 @@
         <v>107</v>
       </c>
       <c r="B98" s="5" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
       <c r="C98" t="s">
         <v>8</v>
@@ -20963,10 +21096,10 @@
     </row>
     <row r="99" spans="1:8">
       <c r="A99" s="4" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
       <c r="B99" s="5" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
       <c r="C99" t="s">
         <v>8</v>
@@ -20989,16 +21122,16 @@
     </row>
     <row r="100" spans="1:8">
       <c r="A100" s="4" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
       <c r="B100" s="5" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
       <c r="C100" t="s">
         <v>8</v>
       </c>
       <c r="D100" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
       <c r="E100" t="s">
         <v>10</v>
@@ -21015,10 +21148,10 @@
     </row>
     <row r="101" spans="1:8">
       <c r="A101" s="4" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
       <c r="B101" s="5" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
       <c r="C101" t="s">
         <v>8</v>
@@ -21041,10 +21174,10 @@
     </row>
     <row r="102" spans="1:8">
       <c r="A102" s="4" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
       <c r="B102" s="5" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
       <c r="C102" t="s">
         <v>8</v>
@@ -21063,6 +21196,422 @@
       </c>
       <c r="H102">
         <v>-92.450855000000004</v>
+      </c>
+    </row>
+    <row r="103" spans="1:8">
+      <c r="A103" s="4" t="s">
+        <v>123</v>
+      </c>
+      <c r="B103" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="C103" t="s">
+        <v>8</v>
+      </c>
+      <c r="D103" t="s">
+        <v>41</v>
+      </c>
+      <c r="E103" t="s">
+        <v>10</v>
+      </c>
+      <c r="F103" t="s">
+        <v>11</v>
+      </c>
+      <c r="G103">
+        <v>42.515762000000002</v>
+      </c>
+      <c r="H103">
+        <v>-92.467191999999997</v>
+      </c>
+    </row>
+    <row r="104" spans="1:8">
+      <c r="A104" s="4" t="s">
+        <v>125</v>
+      </c>
+      <c r="B104" s="5" t="s">
+        <v>126</v>
+      </c>
+      <c r="C104" t="s">
+        <v>8</v>
+      </c>
+      <c r="D104" t="s">
+        <v>41</v>
+      </c>
+      <c r="E104" t="s">
+        <v>10</v>
+      </c>
+      <c r="F104" t="s">
+        <v>11</v>
+      </c>
+      <c r="G104">
+        <v>42.515762000000002</v>
+      </c>
+      <c r="H104">
+        <v>-92.467191999999997</v>
+      </c>
+    </row>
+    <row r="105" spans="1:8">
+      <c r="A105" s="4" t="s">
+        <v>127</v>
+      </c>
+      <c r="B105" s="5" t="s">
+        <v>128</v>
+      </c>
+      <c r="C105" t="s">
+        <v>8</v>
+      </c>
+      <c r="D105" t="s">
+        <v>16</v>
+      </c>
+      <c r="E105" t="s">
+        <v>10</v>
+      </c>
+      <c r="F105" t="s">
+        <v>11</v>
+      </c>
+      <c r="G105">
+        <v>42.514871999999997</v>
+      </c>
+      <c r="H105">
+        <v>-92.458669999999998</v>
+      </c>
+    </row>
+    <row r="106" spans="1:8">
+      <c r="A106" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="B106" s="5" t="s">
+        <v>130</v>
+      </c>
+      <c r="C106" t="s">
+        <v>8</v>
+      </c>
+      <c r="D106" t="s">
+        <v>39</v>
+      </c>
+      <c r="E106" t="s">
+        <v>10</v>
+      </c>
+      <c r="F106" t="s">
+        <v>11</v>
+      </c>
+      <c r="G106">
+        <v>42.517180000000003</v>
+      </c>
+      <c r="H106">
+        <v>-92.461573000000001</v>
+      </c>
+    </row>
+    <row r="107" spans="1:8">
+      <c r="A107" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B107" s="5" t="s">
+        <v>132</v>
+      </c>
+      <c r="C107" t="s">
+        <v>8</v>
+      </c>
+      <c r="D107" t="s">
+        <v>25</v>
+      </c>
+      <c r="E107" t="s">
+        <v>10</v>
+      </c>
+      <c r="F107" t="s">
+        <v>11</v>
+      </c>
+      <c r="G107">
+        <v>42.511991000000002</v>
+      </c>
+      <c r="H107">
+        <v>-92.463426999999996</v>
+      </c>
+    </row>
+    <row r="108" spans="1:8">
+      <c r="A108" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="B108" s="5" t="s">
+        <v>133</v>
+      </c>
+      <c r="C108" t="s">
+        <v>8</v>
+      </c>
+      <c r="D108" t="s">
+        <v>35</v>
+      </c>
+      <c r="E108" t="s">
+        <v>10</v>
+      </c>
+      <c r="F108" t="s">
+        <v>11</v>
+      </c>
+      <c r="G108">
+        <v>42.518351000000003</v>
+      </c>
+      <c r="H108">
+        <v>-92.462954999999994</v>
+      </c>
+    </row>
+    <row r="109" spans="1:8">
+      <c r="A109" s="4" t="s">
+        <v>135</v>
+      </c>
+      <c r="B109" s="5" t="s">
+        <v>136</v>
+      </c>
+      <c r="C109" t="s">
+        <v>8</v>
+      </c>
+      <c r="D109" t="s">
+        <v>134</v>
+      </c>
+      <c r="E109" t="s">
+        <v>10</v>
+      </c>
+      <c r="F109" t="s">
+        <v>11</v>
+      </c>
+      <c r="G109">
+        <v>42.513953000000001</v>
+      </c>
+      <c r="H109">
+        <v>-92.461827999999997</v>
+      </c>
+    </row>
+    <row r="110" spans="1:8">
+      <c r="A110" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B110" s="5" t="s">
+        <v>138</v>
+      </c>
+      <c r="C110" t="s">
+        <v>8</v>
+      </c>
+      <c r="D110" t="s">
+        <v>40</v>
+      </c>
+      <c r="E110" t="s">
+        <v>10</v>
+      </c>
+      <c r="F110" t="s">
+        <v>11</v>
+      </c>
+      <c r="G110">
+        <v>42.517180000000003</v>
+      </c>
+      <c r="H110">
+        <v>-92.466530000000006</v>
+      </c>
+    </row>
+    <row r="111" spans="1:8">
+      <c r="A111" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="B111" s="5" t="s">
+        <v>139</v>
+      </c>
+      <c r="C111" t="s">
+        <v>8</v>
+      </c>
+      <c r="D111" t="s">
+        <v>36</v>
+      </c>
+      <c r="E111" t="s">
+        <v>10</v>
+      </c>
+      <c r="F111" t="s">
+        <v>11</v>
+      </c>
+      <c r="G111">
+        <v>42.518335</v>
+      </c>
+      <c r="H111">
+        <v>-92.461462999999995</v>
+      </c>
+    </row>
+    <row r="112" spans="1:8">
+      <c r="A112" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="B112" s="5" t="s">
+        <v>141</v>
+      </c>
+      <c r="C112" t="s">
+        <v>32</v>
+      </c>
+      <c r="D112" t="s">
+        <v>28</v>
+      </c>
+      <c r="E112" t="s">
+        <v>10</v>
+      </c>
+      <c r="F112" t="s">
+        <v>11</v>
+      </c>
+      <c r="G112">
+        <v>42.512656</v>
+      </c>
+      <c r="H112">
+        <v>-92.467299999999994</v>
+      </c>
+    </row>
+    <row r="113" spans="1:8">
+      <c r="A113" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B113" s="5" t="s">
+        <v>143</v>
+      </c>
+      <c r="C113" t="s">
+        <v>37</v>
+      </c>
+      <c r="D113" t="s">
+        <v>49</v>
+      </c>
+      <c r="E113" t="s">
+        <v>13</v>
+      </c>
+      <c r="F113" t="s">
+        <v>11</v>
+      </c>
+      <c r="G113">
+        <v>42.507286000000001</v>
+      </c>
+      <c r="H113">
+        <v>-92.453878000000003</v>
+      </c>
+    </row>
+    <row r="114" spans="1:8">
+      <c r="A114" s="4" t="s">
+        <v>144</v>
+      </c>
+      <c r="B114" s="5" t="s">
+        <v>145</v>
+      </c>
+      <c r="C114" t="s">
+        <v>37</v>
+      </c>
+      <c r="D114" t="s">
+        <v>36</v>
+      </c>
+      <c r="E114" t="s">
+        <v>10</v>
+      </c>
+      <c r="F114" t="s">
+        <v>11</v>
+      </c>
+      <c r="G114">
+        <v>42.518335</v>
+      </c>
+      <c r="H114">
+        <v>-92.461462999999995</v>
+      </c>
+    </row>
+    <row r="115" spans="1:8">
+      <c r="A115" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B115" s="5" t="s">
+        <v>160</v>
+      </c>
+      <c r="C115" t="s">
+        <v>8</v>
+      </c>
+      <c r="D115" t="s">
+        <v>36</v>
+      </c>
+      <c r="E115" t="s">
+        <v>10</v>
+      </c>
+      <c r="F115" t="s">
+        <v>11</v>
+      </c>
+      <c r="G115">
+        <v>42.518335</v>
+      </c>
+      <c r="H115">
+        <v>-92.461462999999995</v>
+      </c>
+    </row>
+    <row r="116" spans="1:8">
+      <c r="A116" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="B116" s="5" t="s">
+        <v>161</v>
+      </c>
+      <c r="C116" t="s">
+        <v>8</v>
+      </c>
+      <c r="D116" t="s">
+        <v>149</v>
+      </c>
+      <c r="E116" t="s">
+        <v>10</v>
+      </c>
+      <c r="F116" t="s">
+        <v>11</v>
+      </c>
+      <c r="G116">
+        <v>42.513128999999999</v>
+      </c>
+      <c r="H116">
+        <v>-92.465681000000004</v>
+      </c>
+    </row>
+    <row r="117" spans="1:8">
+      <c r="A117" s="4" t="s">
+        <v>162</v>
+      </c>
+      <c r="B117" s="5" t="s">
+        <v>163</v>
+      </c>
+      <c r="C117" t="s">
+        <v>8</v>
+      </c>
+      <c r="D117" t="s">
+        <v>42</v>
+      </c>
+      <c r="E117" t="s">
+        <v>10</v>
+      </c>
+      <c r="F117" t="s">
+        <v>11</v>
+      </c>
+      <c r="G117">
+        <v>42.514471</v>
+      </c>
+      <c r="H117">
+        <v>-92.459536</v>
+      </c>
+    </row>
+    <row r="118" spans="1:8">
+      <c r="A118" s="4" t="s">
+        <v>164</v>
+      </c>
+      <c r="B118" s="5" t="s">
+        <v>165</v>
+      </c>
+      <c r="C118" t="s">
+        <v>8</v>
+      </c>
+      <c r="D118" t="s">
+        <v>45</v>
+      </c>
+      <c r="E118" t="s">
+        <v>10</v>
+      </c>
+      <c r="F118" t="s">
+        <v>11</v>
+      </c>
+      <c r="G118">
+        <v>42.511201</v>
+      </c>
+      <c r="H118">
+        <v>-92.464398000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>